<commit_message>
created covid corner database tables
</commit_message>
<xml_diff>
--- a/Covid_Corner_App.xlsx
+++ b/Covid_Corner_App.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\Covid Corner\Covid-Corner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA4CE36-24D2-4062-AFCD-91C7FF2081B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB672F7-C90E-4B1F-8A07-A64ADE97866B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F2770DF9-C8D8-4148-8A2E-B1950FA71620}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2770DF9-C8D8-4148-8A2E-B1950FA71620}"/>
   </bookViews>
   <sheets>
     <sheet name="In words" sheetId="1" r:id="rId1"/>
     <sheet name="Graphical" sheetId="2" r:id="rId2"/>
+    <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Users">Lists!$A$1:$A$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,82 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
-  <si>
-    <t>App with sections for</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
-    <t>Companies</t>
-  </si>
-  <si>
-    <t>Doctors</t>
-  </si>
-  <si>
-    <t>Functionality</t>
-  </si>
-  <si>
-    <t>Choose to 'opt-in' when walking into a company (preferably by wifi)</t>
-  </si>
-  <si>
-    <t>Option to display add</t>
-  </si>
-  <si>
-    <t>Pay x per visit/add</t>
-  </si>
-  <si>
-    <t>Get a unique VISIT_ID for each visit</t>
-  </si>
-  <si>
-    <t>Turn all VISIT_ID's into INFECTED_ID's once tested positive</t>
-  </si>
-  <si>
-    <t>Find STORE_ID's for all INFECTED_ID's</t>
-  </si>
-  <si>
-    <t>Register DATE &amp; TIME of infection</t>
-  </si>
-  <si>
-    <t>Find all VISIT_ID's of others after INFECTED_ID's time of visit</t>
-  </si>
-  <si>
-    <t>Flag those VISIT_ID's so that next time they open the app they are now AT_RISK_ID</t>
-  </si>
-  <si>
-    <t>VISIT_ID</t>
-  </si>
-  <si>
-    <t>INFECTED_ID</t>
-  </si>
-  <si>
-    <t>COMPANY_ID</t>
-  </si>
-  <si>
-    <t>Register and received a unique store locator (COMPANY_ID)</t>
-  </si>
-  <si>
-    <t>DOCTOR_KEY</t>
-  </si>
-  <si>
-    <t>Register in order to obtain key to confirm positive case as key to user releasing information through DOCTOR_KEY</t>
-  </si>
-  <si>
-    <t>When someone tests positive</t>
-  </si>
-  <si>
-    <t>Turn list of that person's VISIT_ID's into INFECTED_ID's (maybe with DOCTOR_ID-key)</t>
-  </si>
-  <si>
-    <t>AT_RISK_FLAG</t>
-  </si>
-  <si>
-    <t>Update database VISIT_ID's of all that were within time between visit and set AT_RISK_FLAG</t>
-  </si>
-  <si>
-    <t>Next time user looks at his/her VISIT_ID list, some may have AT_RISK_FLAG displayed (and optionally COMPANY_ID and time between that VISIT_ID and INFECTED_ID)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>1. SYSTEM SETTINGS</t>
   </si>
@@ -158,6 +86,193 @@
   </si>
   <si>
     <t>7. COVID NEAR ME</t>
+  </si>
+  <si>
+    <t>1A1</t>
+  </si>
+  <si>
+    <t>1A2</t>
+  </si>
+  <si>
+    <t>1A3</t>
+  </si>
+  <si>
+    <t>Location Service (Check 1A1)
+* Never/Manually 
+* When using the app
+* Always</t>
+  </si>
+  <si>
+    <t>Notifications (Toggle 1A2)
+* On/Off (On &gt; Register)</t>
+  </si>
+  <si>
+    <t>Time of Overlap (Slider 1A3):
+* Hours between Infected Visit and Personal visit log</t>
+  </si>
+  <si>
+    <t>Building Block</t>
+  </si>
+  <si>
+    <t>Deliverable</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Aukje</t>
+  </si>
+  <si>
+    <t>Define COMPANY_ID's  (dropdown list 1B1) 
+* Register &amp; obtain 
+* Precreated in Database</t>
+  </si>
+  <si>
+    <t>1B1</t>
+  </si>
+  <si>
+    <t>Delete options (check 1D1)
+* Variable in days OR
+* Auto after 4 weeks OR
+* Don't delete</t>
+  </si>
+  <si>
+    <t>1B2</t>
+  </si>
+  <si>
+    <t>Create log entry initiated by (2A1):
+* User &gt; Manually
+* Phone &gt; Automatically (Location service ON)
+* Store Initiated &gt; WIFI / Popup &gt; Accept/Decline</t>
+  </si>
+  <si>
+    <t>2A1</t>
+  </si>
+  <si>
+    <t>VISIT_ID Composition (2B1)
+* COMPANY_ID (8 CHAR)
+* DATE TIME stamp (14 CHAR)
+* UNIQUE ID (12 CHAR)</t>
+  </si>
+  <si>
+    <t>2B1</t>
+  </si>
+  <si>
+    <t>view log screen (2C1)
+* Companies and Datetime visited
+* Current Risk Flag
+* Requires 'refresh' and connect to database</t>
+  </si>
+  <si>
+    <t>2C1</t>
+  </si>
+  <si>
+    <t>Process on User side (3A1)
+* User tests positive 
+* User receives DOCTOR_KEY  
+* User sends ALERT to database</t>
+  </si>
+  <si>
+    <t>3A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process on Database side (3B1)
+* Program creates entries in INFECTED_COMPANIES table for all VISIT_ID's user has sent to database </t>
+  </si>
+  <si>
+    <t>3B1</t>
+  </si>
+  <si>
+    <t>Process on App side (3C1)
+* If Push notifactions are on User receives warning in case of 'OVERLAP'
+* If Push notifications are NOT on, app will connect regularly to check for 'OVERLAP'</t>
+  </si>
+  <si>
+    <t>3C1</t>
+  </si>
+  <si>
+    <t>Improve Risk Calculator (4A1)
+* Find better Dataset
+* Create more features  
+* Create &amp; Save new models
+* Integrate into Application</t>
+  </si>
+  <si>
+    <t>4A1</t>
+  </si>
+  <si>
+    <t>Improve Charts (5A1)
+* Add chart by ZIP code</t>
+  </si>
+  <si>
+    <t>5A1</t>
+  </si>
+  <si>
+    <t>Improve Predictions (6A1)
+* Find better Prediction Model
+* Apply to Predictions Page
+* Automate Launch
+* Let user set days out and run</t>
+  </si>
+  <si>
+    <t>6A1</t>
+  </si>
+  <si>
+    <t>Create a new page (7A1)
+* Use User's location
+* Locate infected Companies through Infected_Companies table in app</t>
+  </si>
+  <si>
+    <t>7A1</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Files involved</t>
+  </si>
+  <si>
+    <t>Covid_App.html
+app.js</t>
+  </si>
+  <si>
+    <t>visit_ids.csv
+delete.js (new)</t>
+  </si>
+  <si>
+    <t>visit_ids.csv
+create.js (new)</t>
+  </si>
+  <si>
+    <t>COVID_db
+get_companies.sql
+app.py (FLASK)</t>
+  </si>
+  <si>
+    <t>get_visit_id.py</t>
+  </si>
+  <si>
+    <t>visit_ids.csv
+app.js
+Covid_App.html</t>
   </si>
 </sst>
 </file>
@@ -176,14 +291,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -216,6 +323,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,32 +378,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -299,37 +436,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4067,137 +4197,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E069E1-D9F8-4C5C-AEA4-4FDF3C6F0895}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="32"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
-        <v>24</v>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" t="s">
-        <v>7</v>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
+    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>21</v>
+    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>13</v>
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5F8470F-4617-4DA2-9CDF-30CD632903C5}">
+          <x14:formula1>
+            <xm:f>Lists!$A$2:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7B101A2-19C2-4F8D-955E-373D2A0A89DE}">
+          <x14:formula1>
+            <xm:f>Lists!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4205,154 +4471,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BB704F-0651-4AA1-B509-9078893EE30B}">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="8.88671875" style="15"/>
-    <col min="6" max="11" width="8.88671875" style="16"/>
-    <col min="12" max="12" width="8.88671875" style="17"/>
+    <col min="5" max="5" width="8.88671875" style="14"/>
+    <col min="6" max="11" width="8.88671875" style="15"/>
+    <col min="12" max="12" width="8.88671875" style="16"/>
     <col min="13" max="13" width="4.21875" customWidth="1"/>
-    <col min="14" max="14" width="23.88671875" style="26" customWidth="1"/>
-    <col min="15" max="15" width="10.109375" style="16" customWidth="1"/>
-    <col min="16" max="16" width="23.88671875" style="28" customWidth="1"/>
-    <col min="17" max="17" width="10.109375" style="16" customWidth="1"/>
-    <col min="18" max="18" width="23.88671875" style="28" customWidth="1"/>
-    <col min="19" max="19" width="4.44140625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="23.88671875" style="20" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" style="15" customWidth="1"/>
+    <col min="16" max="16" width="23.88671875" style="22" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" style="15" customWidth="1"/>
+    <col min="18" max="18" width="23.88671875" style="22" customWidth="1"/>
+    <col min="19" max="19" width="4.44140625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="20"/>
+      <c r="A1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="28"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="20"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="28"/>
     </row>
-    <row r="3" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="30"/>
-      <c r="U3" s="24" t="s">
-        <v>39</v>
+    <row r="3" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+      <c r="N3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="18"/>
+      <c r="P3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="24"/>
+      <c r="U3" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
-      <c r="N4" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="31"/>
-      <c r="U4" s="6" t="s">
-        <v>40</v>
+    <row r="4" spans="1:28" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
+      <c r="N4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="25"/>
+      <c r="U4" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="D6" s="5"/>
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4364,4 +4630,54 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E9FAD9-C137-47CD-A6F0-B2DBA63995B9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>